<commit_message>
attempt to add todo list
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosta\OneDrive\Desktop\dashboard V.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\dashboard-V.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9DF7F3-203F-49BE-BDE0-67DFB641C642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6EE956-CE8F-4ADA-9690-E7773456198E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -670,10 +670,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}" name="Table22" displayName="Table22" ref="G3:J71" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="G3:J71" xr:uid="{9A42150A-74BB-4659-8BE3-C38AE4DF6F2F}"/>
@@ -993,7 +989,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -1077,11 +1073,11 @@
       <c r="D2" s="17"/>
       <c r="E2" s="6">
         <f ca="1">(E3+(F3/60))/60</f>
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="7">
         <f ca="1">(E3+(F3/60))</f>
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
@@ -1135,7 +1131,7 @@
       </c>
       <c r="E3" s="8">
         <f ca="1">SUMIF(Table223[CHECK],"Done",E$4:E$60)</f>
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F3" s="8">
         <f ca="1">SUMIF(Table223[CHECK],"Done",F$4:F$60)</f>
@@ -1223,7 +1219,7 @@
       </c>
       <c r="G4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45391</v>
+        <v>45393</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -1256,7 +1252,7 @@
       </c>
       <c r="S4" s="15">
         <f ca="1">TODAY()</f>
-        <v>45391</v>
+        <v>45393</v>
       </c>
       <c r="T4" s="1">
         <v>0</v>
@@ -1290,7 +1286,7 @@
       </c>
       <c r="G5" s="15">
         <f ca="1">G4+1</f>
-        <v>45392</v>
+        <v>45394</v>
       </c>
       <c r="H5" s="1">
         <v>2.0833333333333333E-3</v>
@@ -1324,7 +1320,7 @@
       </c>
       <c r="S5" s="15">
         <f ca="1">S4+1</f>
-        <v>45392</v>
+        <v>45394</v>
       </c>
       <c r="T5" s="1">
         <v>1.0416666666666667E-3</v>
@@ -1358,7 +1354,7 @@
       </c>
       <c r="G6" s="15">
         <f t="shared" ref="G6:G69" ca="1" si="1">G5+1</f>
-        <v>45393</v>
+        <v>45395</v>
       </c>
       <c r="H6" s="1">
         <v>4.1666666666666701E-3</v>
@@ -1392,7 +1388,7 @@
       </c>
       <c r="S6" s="15">
         <f t="shared" ref="S6:S61" ca="1" si="3">S5+1</f>
-        <v>45393</v>
+        <v>45395</v>
       </c>
       <c r="T6" s="1">
         <v>2.0833333333333298E-3</v>
@@ -1415,7 +1411,9 @@
       <c r="C7" s="1">
         <v>8.3333333333333402E-3</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E7" s="2">
         <v>3</v>
       </c>
@@ -1424,7 +1422,7 @@
       </c>
       <c r="G7" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45394</v>
+        <v>45396</v>
       </c>
       <c r="H7" s="1">
         <v>6.2500000000000003E-3</v>
@@ -1458,7 +1456,7 @@
       </c>
       <c r="S7" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45394</v>
+        <v>45396</v>
       </c>
       <c r="T7" s="1">
         <v>3.1250000000000002E-3</v>
@@ -1481,7 +1479,9 @@
       <c r="C8" s="1">
         <v>1.0416666666666701E-2</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E8" s="2">
         <v>3</v>
       </c>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="G8" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45395</v>
+        <v>45397</v>
       </c>
       <c r="H8" s="1">
         <v>8.3333333333333297E-3</v>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="S8" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45395</v>
+        <v>45397</v>
       </c>
       <c r="T8" s="1">
         <v>4.1666666666666701E-3</v>
@@ -1547,7 +1547,9 @@
       <c r="C9" s="1">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E9" s="2">
         <v>3</v>
       </c>
@@ -1556,7 +1558,7 @@
       </c>
       <c r="G9" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45396</v>
+        <v>45398</v>
       </c>
       <c r="H9" s="1">
         <v>1.0416666666666701E-2</v>
@@ -1590,7 +1592,7 @@
       </c>
       <c r="S9" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45396</v>
+        <v>45398</v>
       </c>
       <c r="T9" s="1">
         <v>5.2083333333333296E-3</v>
@@ -1613,7 +1615,9 @@
       <c r="C10" s="1">
         <v>1.4583333333333301E-2</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E10" s="2">
         <v>3</v>
       </c>
@@ -1622,7 +1626,7 @@
       </c>
       <c r="G10" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45397</v>
+        <v>45399</v>
       </c>
       <c r="H10" s="1">
         <v>1.2500000000000001E-2</v>
@@ -1656,7 +1660,7 @@
       </c>
       <c r="S10" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45397</v>
+        <v>45399</v>
       </c>
       <c r="T10" s="1">
         <v>6.2500000000000003E-3</v>
@@ -1679,7 +1683,9 @@
       <c r="C11" s="1">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E11" s="2">
         <v>3</v>
       </c>
@@ -1688,7 +1694,7 @@
       </c>
       <c r="G11" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45398</v>
+        <v>45400</v>
       </c>
       <c r="H11" s="1">
         <v>1.4583333333333301E-2</v>
@@ -1722,7 +1728,7 @@
       </c>
       <c r="S11" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45398</v>
+        <v>45400</v>
       </c>
       <c r="T11" s="1">
         <v>7.2916666666666703E-3</v>
@@ -1745,7 +1751,9 @@
       <c r="C12" s="1">
         <v>1.8749999999999999E-2</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E12" s="2">
         <v>3</v>
       </c>
@@ -1754,7 +1762,7 @@
       </c>
       <c r="G12" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45399</v>
+        <v>45401</v>
       </c>
       <c r="H12" s="1">
         <v>1.6666666666666701E-2</v>
@@ -1788,7 +1796,7 @@
       </c>
       <c r="S12" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45399</v>
+        <v>45401</v>
       </c>
       <c r="T12" s="1">
         <v>8.3333333333333297E-3</v>
@@ -1811,7 +1819,9 @@
       <c r="C13" s="1">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E13" s="2">
         <v>3</v>
       </c>
@@ -1820,7 +1830,7 @@
       </c>
       <c r="G13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45400</v>
+        <v>45402</v>
       </c>
       <c r="H13" s="1">
         <v>1.8749999999999999E-2</v>
@@ -1854,7 +1864,7 @@
       </c>
       <c r="S13" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45400</v>
+        <v>45402</v>
       </c>
       <c r="T13" s="1">
         <v>9.3749999999999997E-3</v>
@@ -1875,7 +1885,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="H14" s="1">
         <v>2.0833333333333301E-2</v>
@@ -1909,7 +1919,7 @@
       </c>
       <c r="S14" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="T14" s="1">
         <v>1.0416666666666701E-2</v>
@@ -1930,7 +1940,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45402</v>
+        <v>45404</v>
       </c>
       <c r="H15" s="1">
         <v>2.29166666666667E-2</v>
@@ -1964,7 +1974,7 @@
       </c>
       <c r="S15" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45402</v>
+        <v>45404</v>
       </c>
       <c r="T15" s="1">
         <v>1.14583333333333E-2</v>
@@ -1985,7 +1995,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45403</v>
+        <v>45405</v>
       </c>
       <c r="H16" s="1">
         <v>2.5000000000000001E-2</v>
@@ -2019,7 +2029,7 @@
       </c>
       <c r="S16" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45403</v>
+        <v>45405</v>
       </c>
       <c r="T16" s="1">
         <v>1.2500000000000001E-2</v>
@@ -2040,7 +2050,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="H17" s="1">
         <v>2.70833333333333E-2</v>
@@ -2074,7 +2084,7 @@
       </c>
       <c r="S17" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="T17" s="1">
         <v>1.35416666666667E-2</v>
@@ -2095,7 +2105,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45405</v>
+        <v>45407</v>
       </c>
       <c r="H18" s="1">
         <v>2.9166666666666698E-2</v>
@@ -2129,7 +2139,7 @@
       </c>
       <c r="S18" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45405</v>
+        <v>45407</v>
       </c>
       <c r="T18" s="1">
         <v>1.4583333333333301E-2</v>
@@ -2150,7 +2160,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="H19" s="1">
         <v>3.125E-2</v>
@@ -2184,7 +2194,7 @@
       </c>
       <c r="S19" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="T19" s="1">
         <v>1.5625E-2</v>
@@ -2205,7 +2215,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45407</v>
+        <v>45409</v>
       </c>
       <c r="H20" s="1">
         <v>3.3333333333333298E-2</v>
@@ -2239,7 +2249,7 @@
       </c>
       <c r="S20" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45407</v>
+        <v>45409</v>
       </c>
       <c r="T20" s="1">
         <v>1.6666666666666701E-2</v>
@@ -2260,7 +2270,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45408</v>
+        <v>45410</v>
       </c>
       <c r="H21" s="1">
         <v>3.54166666666667E-2</v>
@@ -2294,7 +2304,7 @@
       </c>
       <c r="S21" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45408</v>
+        <v>45410</v>
       </c>
       <c r="T21" s="1">
         <v>1.7708333333333302E-2</v>
@@ -2315,7 +2325,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45409</v>
+        <v>45411</v>
       </c>
       <c r="H22" s="1">
         <v>3.7499999999999999E-2</v>
@@ -2349,7 +2359,7 @@
       </c>
       <c r="S22" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45409</v>
+        <v>45411</v>
       </c>
       <c r="T22" s="1">
         <v>1.8749999999999999E-2</v>
@@ -2370,7 +2380,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45410</v>
+        <v>45412</v>
       </c>
       <c r="H23" s="1">
         <v>3.9583333333333297E-2</v>
@@ -2400,7 +2410,7 @@
       <c r="R23" s="2"/>
       <c r="S23" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45410</v>
+        <v>45412</v>
       </c>
       <c r="T23" s="1">
         <v>1.97916666666667E-2</v>
@@ -2421,7 +2431,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45411</v>
+        <v>45413</v>
       </c>
       <c r="H24" s="1">
         <v>4.1666666666666699E-2</v>
@@ -2451,7 +2461,7 @@
       <c r="R24" s="2"/>
       <c r="S24" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45411</v>
+        <v>45413</v>
       </c>
       <c r="T24" s="1">
         <v>2.0833333333333301E-2</v>
@@ -2472,7 +2482,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="H25" s="1">
         <v>4.3749999999999997E-2</v>
@@ -2502,7 +2512,7 @@
       <c r="R25" s="2"/>
       <c r="S25" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="T25" s="1">
         <v>2.1874999999999999E-2</v>
@@ -2523,7 +2533,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45413</v>
+        <v>45415</v>
       </c>
       <c r="H26" s="1">
         <v>4.5833333333333302E-2</v>
@@ -2553,7 +2563,7 @@
       <c r="R26" s="2"/>
       <c r="S26" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45413</v>
+        <v>45415</v>
       </c>
       <c r="T26" s="1">
         <v>2.29166666666667E-2</v>
@@ -2574,7 +2584,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45414</v>
+        <v>45416</v>
       </c>
       <c r="H27" s="1">
         <v>4.7916666666666698E-2</v>
@@ -2604,7 +2614,7 @@
       <c r="R27" s="2"/>
       <c r="S27" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45414</v>
+        <v>45416</v>
       </c>
       <c r="T27" s="1">
         <v>2.39583333333333E-2</v>
@@ -2625,7 +2635,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45415</v>
+        <v>45417</v>
       </c>
       <c r="H28" s="1">
         <v>0.05</v>
@@ -2655,7 +2665,7 @@
       <c r="R28" s="2"/>
       <c r="S28" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45415</v>
+        <v>45417</v>
       </c>
       <c r="T28" s="1">
         <v>2.5000000000000001E-2</v>
@@ -2676,7 +2686,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45416</v>
+        <v>45418</v>
       </c>
       <c r="H29" s="1">
         <v>5.2083333333333301E-2</v>
@@ -2706,7 +2716,7 @@
       <c r="R29" s="2"/>
       <c r="S29" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45416</v>
+        <v>45418</v>
       </c>
       <c r="T29" s="1">
         <v>2.6041666666666699E-2</v>
@@ -2727,7 +2737,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45417</v>
+        <v>45419</v>
       </c>
       <c r="H30" s="1">
         <v>5.4166666666666703E-2</v>
@@ -2757,7 +2767,7 @@
       <c r="R30" s="2"/>
       <c r="S30" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45417</v>
+        <v>45419</v>
       </c>
       <c r="T30" s="1">
         <v>2.70833333333333E-2</v>
@@ -2778,7 +2788,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45418</v>
+        <v>45420</v>
       </c>
       <c r="H31" s="1">
         <v>5.6250000000000001E-2</v>
@@ -2808,7 +2818,7 @@
       <c r="R31" s="2"/>
       <c r="S31" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45418</v>
+        <v>45420</v>
       </c>
       <c r="T31" s="1">
         <v>2.8125000000000001E-2</v>
@@ -2829,7 +2839,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="H32" s="1">
         <v>5.83333333333333E-2</v>
@@ -2859,7 +2869,7 @@
       <c r="R32" s="2"/>
       <c r="S32" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="T32" s="1">
         <v>2.9166666666666698E-2</v>
@@ -2880,7 +2890,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45420</v>
+        <v>45422</v>
       </c>
       <c r="H33" s="1">
         <v>6.0416666666666702E-2</v>
@@ -2910,7 +2920,7 @@
       <c r="R33" s="2"/>
       <c r="S33" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45420</v>
+        <v>45422</v>
       </c>
       <c r="T33" s="1">
         <v>3.0208333333333299E-2</v>
@@ -2931,7 +2941,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45421</v>
+        <v>45423</v>
       </c>
       <c r="H34" s="1">
         <v>6.25E-2</v>
@@ -2961,7 +2971,7 @@
       <c r="R34" s="2"/>
       <c r="S34" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45421</v>
+        <v>45423</v>
       </c>
       <c r="T34" s="1">
         <v>3.125E-2</v>
@@ -2982,7 +2992,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45422</v>
+        <v>45424</v>
       </c>
       <c r="H35" s="1">
         <v>6.4583333333333298E-2</v>
@@ -3012,7 +3022,7 @@
       <c r="R35" s="2"/>
       <c r="S35" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45422</v>
+        <v>45424</v>
       </c>
       <c r="T35" s="1">
         <v>3.2291666666666698E-2</v>
@@ -3033,7 +3043,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45423</v>
+        <v>45425</v>
       </c>
       <c r="H36" s="1">
         <v>6.6666666666666693E-2</v>
@@ -3063,7 +3073,7 @@
       <c r="R36" s="2"/>
       <c r="S36" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45423</v>
+        <v>45425</v>
       </c>
       <c r="T36" s="1">
         <v>3.3333333333333298E-2</v>
@@ -3084,7 +3094,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45424</v>
+        <v>45426</v>
       </c>
       <c r="H37" s="1">
         <v>6.8750000000000006E-2</v>
@@ -3114,7 +3124,7 @@
       <c r="R37" s="2"/>
       <c r="S37" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45424</v>
+        <v>45426</v>
       </c>
       <c r="T37" s="1">
         <v>3.4375000000000003E-2</v>
@@ -3135,7 +3145,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45425</v>
+        <v>45427</v>
       </c>
       <c r="H38" s="1">
         <v>7.0833333333333304E-2</v>
@@ -3165,7 +3175,7 @@
       <c r="R38" s="2"/>
       <c r="S38" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45425</v>
+        <v>45427</v>
       </c>
       <c r="T38" s="1">
         <v>3.54166666666667E-2</v>
@@ -3186,7 +3196,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45426</v>
+        <v>45428</v>
       </c>
       <c r="H39" s="1">
         <v>7.2916666666666699E-2</v>
@@ -3216,7 +3226,7 @@
       <c r="R39" s="2"/>
       <c r="S39" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45426</v>
+        <v>45428</v>
       </c>
       <c r="T39" s="1">
         <v>3.6458333333333301E-2</v>
@@ -3237,7 +3247,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45427</v>
+        <v>45429</v>
       </c>
       <c r="H40" s="1">
         <v>7.4999999999999997E-2</v>
@@ -3267,7 +3277,7 @@
       <c r="R40" s="2"/>
       <c r="S40" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45427</v>
+        <v>45429</v>
       </c>
       <c r="T40" s="1">
         <v>3.7499999999999999E-2</v>
@@ -3288,7 +3298,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45428</v>
+        <v>45430</v>
       </c>
       <c r="H41" s="1">
         <v>7.7083333333333295E-2</v>
@@ -3314,7 +3324,7 @@
       <c r="R41" s="2"/>
       <c r="S41" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45428</v>
+        <v>45430</v>
       </c>
       <c r="T41" s="1">
         <v>3.8541666666666703E-2</v>
@@ -3335,7 +3345,7 @@
       <c r="F42" s="2"/>
       <c r="G42" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45429</v>
+        <v>45431</v>
       </c>
       <c r="H42" s="1">
         <v>7.9166666666666705E-2</v>
@@ -3361,7 +3371,7 @@
       <c r="R42" s="2"/>
       <c r="S42" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45429</v>
+        <v>45431</v>
       </c>
       <c r="T42" s="1">
         <v>3.9583333333333297E-2</v>
@@ -3382,7 +3392,7 @@
       <c r="F43" s="2"/>
       <c r="G43" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45430</v>
+        <v>45432</v>
       </c>
       <c r="H43" s="1">
         <v>8.1250000000000003E-2</v>
@@ -3408,7 +3418,7 @@
       <c r="R43" s="2"/>
       <c r="S43" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45430</v>
+        <v>45432</v>
       </c>
       <c r="T43" s="1">
         <v>4.1666666666666664E-2</v>
@@ -3429,7 +3439,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45431</v>
+        <v>45433</v>
       </c>
       <c r="H44" s="1">
         <v>8.3333333333333301E-2</v>
@@ -3455,7 +3465,7 @@
       <c r="R44" s="2"/>
       <c r="S44" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45431</v>
+        <v>45433</v>
       </c>
       <c r="T44" s="1">
         <v>4.5833333333333302E-2</v>
@@ -3476,7 +3486,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45432</v>
+        <v>45434</v>
       </c>
       <c r="H45" s="1">
         <v>8.5416666666666696E-2</v>
@@ -3502,7 +3512,7 @@
       <c r="R45" s="2"/>
       <c r="S45" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45432</v>
+        <v>45434</v>
       </c>
       <c r="T45" s="1">
         <v>4.9999999999999899E-2</v>
@@ -3523,7 +3533,7 @@
       <c r="F46" s="2"/>
       <c r="G46" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45433</v>
+        <v>45435</v>
       </c>
       <c r="H46" s="1">
         <v>8.7499999999999994E-2</v>
@@ -3549,7 +3559,7 @@
       <c r="R46" s="2"/>
       <c r="S46" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45433</v>
+        <v>45435</v>
       </c>
       <c r="T46" s="1">
         <v>5.4166666666666599E-2</v>
@@ -3570,7 +3580,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45434</v>
+        <v>45436</v>
       </c>
       <c r="H47" s="1">
         <v>8.9583333333333307E-2</v>
@@ -3596,7 +3606,7 @@
       <c r="R47" s="2"/>
       <c r="S47" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45434</v>
+        <v>45436</v>
       </c>
       <c r="T47" s="1">
         <v>5.83333333333333E-2</v>
@@ -3617,7 +3627,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45435</v>
+        <v>45437</v>
       </c>
       <c r="H48" s="1">
         <v>9.1666666666666702E-2</v>
@@ -3643,7 +3653,7 @@
       <c r="R48" s="2"/>
       <c r="S48" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45435</v>
+        <v>45437</v>
       </c>
       <c r="T48" s="1">
         <v>6.2499999999999903E-2</v>
@@ -3664,7 +3674,7 @@
       <c r="F49" s="2"/>
       <c r="G49" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45436</v>
+        <v>45438</v>
       </c>
       <c r="H49" s="1">
         <v>9.375E-2</v>
@@ -3690,7 +3700,7 @@
       <c r="R49" s="2"/>
       <c r="S49" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45436</v>
+        <v>45438</v>
       </c>
       <c r="T49" s="1">
         <v>6.6666666666666499E-2</v>
@@ -3711,7 +3721,7 @@
       <c r="F50" s="2"/>
       <c r="G50" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45437</v>
+        <v>45439</v>
       </c>
       <c r="H50" s="1">
         <v>9.5833333333333298E-2</v>
@@ -3737,7 +3747,7 @@
       <c r="R50" s="2"/>
       <c r="S50" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45437</v>
+        <v>45439</v>
       </c>
       <c r="T50" s="1">
         <v>7.0833333333333207E-2</v>
@@ -3758,7 +3768,7 @@
       <c r="F51" s="2"/>
       <c r="G51" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45438</v>
+        <v>45440</v>
       </c>
       <c r="H51" s="1">
         <v>9.7916666666666693E-2</v>
@@ -3784,7 +3794,7 @@
       <c r="R51" s="2"/>
       <c r="S51" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45438</v>
+        <v>45440</v>
       </c>
       <c r="T51" s="1">
         <v>7.4999999999999803E-2</v>
@@ -3805,7 +3815,7 @@
       <c r="F52" s="2"/>
       <c r="G52" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45439</v>
+        <v>45441</v>
       </c>
       <c r="H52" s="1">
         <v>0.1</v>
@@ -3831,7 +3841,7 @@
       <c r="R52" s="2"/>
       <c r="S52" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45439</v>
+        <v>45441</v>
       </c>
       <c r="T52" s="1">
         <v>7.9166666666666399E-2</v>
@@ -3852,7 +3862,7 @@
       <c r="F53" s="2"/>
       <c r="G53" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45440</v>
+        <v>45442</v>
       </c>
       <c r="H53" s="1">
         <v>0.102083333333333</v>
@@ -3878,7 +3888,7 @@
       <c r="R53" s="2"/>
       <c r="S53" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45440</v>
+        <v>45442</v>
       </c>
       <c r="T53" s="1">
         <v>8.3333333333333107E-2</v>
@@ -3899,7 +3909,7 @@
       <c r="F54" s="2"/>
       <c r="G54" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45441</v>
+        <v>45443</v>
       </c>
       <c r="H54" s="1">
         <v>0.104166666666667</v>
@@ -3925,7 +3935,7 @@
       <c r="R54" s="2"/>
       <c r="S54" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45441</v>
+        <v>45443</v>
       </c>
       <c r="T54" s="1">
         <v>9.0277777777777776E-2</v>
@@ -3946,7 +3956,7 @@
       <c r="F55" s="2"/>
       <c r="G55" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45442</v>
+        <v>45444</v>
       </c>
       <c r="H55" s="1">
         <v>0.10625</v>
@@ -3972,7 +3982,7 @@
       <c r="R55" s="2"/>
       <c r="S55" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45442</v>
+        <v>45444</v>
       </c>
       <c r="T55" s="1">
         <v>9.7222222222222404E-2</v>
@@ -3993,7 +4003,7 @@
       <c r="F56" s="2"/>
       <c r="G56" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45443</v>
+        <v>45445</v>
       </c>
       <c r="H56" s="1">
         <v>0.108333333333333</v>
@@ -4019,7 +4029,7 @@
       <c r="R56" s="2"/>
       <c r="S56" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45443</v>
+        <v>45445</v>
       </c>
       <c r="T56" s="1">
         <v>0.104166666666667</v>
@@ -4040,7 +4050,7 @@
       <c r="F57" s="2"/>
       <c r="G57" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45444</v>
+        <v>45446</v>
       </c>
       <c r="H57" s="1">
         <v>0.110416666666667</v>
@@ -4066,7 +4076,7 @@
       <c r="R57" s="2"/>
       <c r="S57" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45444</v>
+        <v>45446</v>
       </c>
       <c r="T57" s="1">
         <v>0.11111111111111199</v>
@@ -4087,7 +4097,7 @@
       <c r="F58" s="2"/>
       <c r="G58" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45445</v>
+        <v>45447</v>
       </c>
       <c r="H58" s="1">
         <v>0.1125</v>
@@ -4113,7 +4123,7 @@
       <c r="R58" s="2"/>
       <c r="S58" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45445</v>
+        <v>45447</v>
       </c>
       <c r="T58" s="1">
         <v>0.118055555555556</v>
@@ -4134,7 +4144,7 @@
       <c r="F59" s="2"/>
       <c r="G59" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45446</v>
+        <v>45448</v>
       </c>
       <c r="H59" s="1">
         <v>0.114583333333333</v>
@@ -4160,7 +4170,7 @@
       <c r="R59" s="2"/>
       <c r="S59" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45446</v>
+        <v>45448</v>
       </c>
       <c r="T59" s="1">
         <v>0.125000000000001</v>
@@ -4181,7 +4191,7 @@
       <c r="F60" s="2"/>
       <c r="G60" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45447</v>
+        <v>45449</v>
       </c>
       <c r="H60" s="1">
         <v>0.116666666666667</v>
@@ -4207,7 +4217,7 @@
       <c r="R60" s="2"/>
       <c r="S60" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45447</v>
+        <v>45449</v>
       </c>
       <c r="T60" s="1">
         <v>0.131944444444446</v>
@@ -4228,7 +4238,7 @@
       <c r="F61" s="2"/>
       <c r="G61" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45448</v>
+        <v>45450</v>
       </c>
       <c r="H61" s="1">
         <v>0.11874999999999999</v>
@@ -4254,7 +4264,7 @@
       <c r="R61" s="2"/>
       <c r="S61" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>45448</v>
+        <v>45450</v>
       </c>
       <c r="T61" s="1">
         <v>0.138888888888891</v>
@@ -4275,7 +4285,7 @@
       <c r="F62" s="2"/>
       <c r="G62" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45449</v>
+        <v>45451</v>
       </c>
       <c r="H62" s="1">
         <v>0.120833333333333</v>
@@ -4315,7 +4325,7 @@
       <c r="F63" s="2"/>
       <c r="G63" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45450</v>
+        <v>45452</v>
       </c>
       <c r="H63" s="1">
         <v>0.12291666666666699</v>
@@ -4355,7 +4365,7 @@
       <c r="F64" s="2"/>
       <c r="G64" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45451</v>
+        <v>45453</v>
       </c>
       <c r="H64" s="1">
         <v>0.125</v>
@@ -4395,7 +4405,7 @@
       <c r="F65" s="2"/>
       <c r="G65" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45452</v>
+        <v>45454</v>
       </c>
       <c r="H65" s="1">
         <v>0.12708333333333299</v>
@@ -4435,7 +4445,7 @@
       <c r="F66" s="2"/>
       <c r="G66" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45453</v>
+        <v>45455</v>
       </c>
       <c r="H66" s="1">
         <v>0.12916666666666701</v>
@@ -4475,7 +4485,7 @@
       <c r="F67" s="2"/>
       <c r="G67" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45454</v>
+        <v>45456</v>
       </c>
       <c r="H67" s="1">
         <v>0.13125000000000001</v>
@@ -4515,7 +4525,7 @@
       <c r="F68" s="2"/>
       <c r="G68" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45455</v>
+        <v>45457</v>
       </c>
       <c r="H68" s="1">
         <v>0.133333333333333</v>
@@ -4555,7 +4565,7 @@
       <c r="F69" s="2"/>
       <c r="G69" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>45456</v>
+        <v>45458</v>
       </c>
       <c r="H69" s="1">
         <v>0.13541666666666699</v>
@@ -4595,7 +4605,7 @@
       <c r="F70" s="2"/>
       <c r="G70" s="15">
         <f t="shared" ref="G70:G71" ca="1" si="4">G69+1</f>
-        <v>45457</v>
+        <v>45459</v>
       </c>
       <c r="H70" s="1">
         <v>0.13750000000000001</v>
@@ -4635,7 +4645,7 @@
       <c r="F71" s="2"/>
       <c r="G71" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>45458</v>
+        <v>45460</v>
       </c>
       <c r="H71" s="1">
         <v>0.139583333333333</v>

</xml_diff>

<commit_message>
Adding First Todos And chck if remain there after deletion and reinstalling
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosta\OneDrive\Desktop\dashboard-V.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C70E4B2-C429-47FA-82BF-179EF952784D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E28CFA-CB4D-45D0-8957-7CAA8873F2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Learn Next.js 13 With This One Project - TODO LIST</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -986,7 +989,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -1070,11 +1073,11 @@
       <c r="D2" s="17"/>
       <c r="E2" s="6">
         <f ca="1">(E3+(F3/60))/60</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F2" s="7">
         <f ca="1">(E3+(F3/60))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
@@ -1128,7 +1131,7 @@
       </c>
       <c r="E3" s="8">
         <f ca="1">SUMIF(Table223[CHECK],"Done",E$4:E$60)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F3" s="8">
         <f ca="1">SUMIF(Table223[CHECK],"Done",F$4:F$60)</f>
@@ -1197,7 +1200,6 @@
     </row>
     <row r="4" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
-        <f ca="1">TODAY()</f>
         <v>45395</v>
       </c>
       <c r="B4" s="1">
@@ -1206,7 +1208,9 @@
       <c r="C4" s="1">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="2">
         <v>3</v>
       </c>
@@ -1262,7 +1266,7 @@
     </row>
     <row r="5" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
-        <f ca="1">A4+1</f>
+        <f>A4+1</f>
         <v>45396</v>
       </c>
       <c r="B5" s="1">
@@ -1271,7 +1275,9 @@
       <c r="C5" s="1">
         <v>4.1666666666666701E-3</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" s="2">
         <v>3</v>
       </c>
@@ -1328,7 +1334,7 @@
     </row>
     <row r="6" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
-        <f t="shared" ref="A6:A13" ca="1" si="0">A5+1</f>
+        <f t="shared" ref="A6:A13" si="0">A5+1</f>
         <v>45397</v>
       </c>
       <c r="B6" s="1">
@@ -1394,7 +1400,7 @@
     </row>
     <row r="7" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>45398</v>
       </c>
       <c r="B7" s="1">
@@ -1460,7 +1466,7 @@
     </row>
     <row r="8" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>45399</v>
       </c>
       <c r="B8" s="1">
@@ -1526,7 +1532,7 @@
     </row>
     <row r="9" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>45400</v>
       </c>
       <c r="B9" s="1">
@@ -1592,7 +1598,7 @@
     </row>
     <row r="10" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>45401</v>
       </c>
       <c r="B10" s="1">
@@ -1658,7 +1664,7 @@
     </row>
     <row r="11" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>45402</v>
       </c>
       <c r="B11" s="1">
@@ -1724,7 +1730,7 @@
     </row>
     <row r="12" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>45403</v>
       </c>
       <c r="B12" s="1">
@@ -1790,7 +1796,7 @@
     </row>
     <row r="13" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>45404</v>
       </c>
       <c r="B13" s="1">

</xml_diff>